<commit_message>
Still trying to figure out the tables.
</commit_message>
<xml_diff>
--- a/data/weekly-in-season/Template_col.xlsx
+++ b/data/weekly-in-season/Template_col.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ARCHAMBAULTJ\Desktop\GIT\WCVI_Esc_Reports\data\weekly-in-season\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1129E8BF-C050-4BFC-AE43-CFE0997E8609}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EBC86CD-F6A6-49E7-96DE-BC1373E6EC87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="2145" windowWidth="21600" windowHeight="11325" xr2:uid="{F99D452C-1FB1-4D6E-A1CC-342D63B9AD5E}"/>
+    <workbookView xWindow="31740" yWindow="8520" windowWidth="21600" windowHeight="6690" xr2:uid="{F99D452C-1FB1-4D6E-A1CC-342D63B9AD5E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,14 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Area</t>
   </si>
   <si>
-    <t>FN Territory</t>
-  </si>
-  <si>
     <t>System</t>
   </si>
   <si>
@@ -113,22 +110,10 @@
     <t>Dec10-16</t>
   </si>
   <si>
-    <t>Dec 17-23</t>
-  </si>
-  <si>
-    <t>Dec 24-30</t>
-  </si>
-  <si>
-    <t>Jan 1-7</t>
-  </si>
-  <si>
-    <t>Jan 8-14</t>
-  </si>
-  <si>
-    <t>Jan 15-21</t>
-  </si>
-  <si>
-    <t>Est vs 12yr Avg Est</t>
+    <t>FN_Territory</t>
+  </si>
+  <si>
+    <t>Est_vs_12yr_Avg</t>
   </si>
 </sst>
 </file>
@@ -179,7 +164,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -271,21 +256,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="double">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -302,7 +272,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -343,13 +313,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="5" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="5" fillId="0" borderId="3" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -667,113 +631,96 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA06C841-C527-4DFD-89B3-E37C0F9AD8D4}">
-  <dimension ref="A1:AF1"/>
+  <dimension ref="A1:Z1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="Z1" sqref="Z1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:32" ht="23.25" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="23.25" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="L1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="M1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="N1" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="O1" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="P1" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="11" t="s">
+      <c r="Q1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="11" t="s">
+      <c r="R1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="11" t="s">
+      <c r="S1" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="12" t="s">
+      <c r="T1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="6" t="s">
+      <c r="U1" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="8" t="s">
+      <c r="V1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="8" t="s">
+      <c r="W1" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="8" t="s">
+      <c r="X1" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="13" t="s">
+      <c r="Y1" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z1" s="11" t="s">
+      <c r="Z1" s="14" t="s">
         <v>25</v>
-      </c>
-      <c r="AA1" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB1" s="14">
-        <v>45291</v>
-      </c>
-      <c r="AC1" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="AD1" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="AE1" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="AF1" s="16" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>